<commit_message>
started implementing genetic algorithm (generating first population but not finished yet), changed data presenting in excel
</commit_message>
<xml_diff>
--- a/input/Data.xlsx
+++ b/input/Data.xlsx
@@ -4,40 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245"/>
   </bookViews>
   <sheets>
-    <sheet name="City" sheetId="1" r:id="rId1"/>
-    <sheet name="Vehicle" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>M4</t>
-  </si>
-  <si>
-    <t>M5</t>
-  </si>
-  <si>
-    <t>M6</t>
-  </si>
-  <si>
-    <t>M7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>V1</t>
   </si>
@@ -52,6 +29,33 @@
   </si>
   <si>
     <t>V5</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>V0</t>
   </si>
 </sst>
 </file>
@@ -392,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,134 +408,107 @@
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="E4" s="1">
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="E6" s="1">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>10</v>
+      <c r="B8" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5.34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5.43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added geographical coordinates and depot, counted distance in route, changed data presenting in excel again
</commit_message>
<xml_diff>
--- a/input/Data.xlsx
+++ b/input/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>V1</t>
   </si>
@@ -22,40 +22,52 @@
     <t>V2</t>
   </si>
   <si>
-    <t>V3</t>
-  </si>
-  <si>
-    <t>V4</t>
-  </si>
-  <si>
-    <t>V5</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C0</t>
-  </si>
-  <si>
     <t>V0</t>
+  </si>
+  <si>
+    <t>City name</t>
+  </si>
+  <si>
+    <t>City amount</t>
+  </si>
+  <si>
+    <t>City latitude</t>
+  </si>
+  <si>
+    <t>City longitude</t>
+  </si>
+  <si>
+    <t>Vehicle name</t>
+  </si>
+  <si>
+    <t>Vehicle amount</t>
+  </si>
+  <si>
+    <t>Depot latitude</t>
+  </si>
+  <si>
+    <t>Depot longitude</t>
+  </si>
+  <si>
+    <t>Warszawa</t>
+  </si>
+  <si>
+    <t>Lodz</t>
+  </si>
+  <si>
+    <t>Krakow</t>
+  </si>
+  <si>
+    <t>Wroclaw</t>
+  </si>
+  <si>
+    <t>Poznan</t>
+  </si>
+  <si>
+    <t>Katowice</t>
+  </si>
+  <si>
+    <t>City name of depot</t>
   </si>
 </sst>
 </file>
@@ -92,9 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -396,119 +409,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="1">
+        <v>51.77</v>
+      </c>
+      <c r="D2" s="1">
+        <v>19.46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1">
+        <v>52.26</v>
+      </c>
+      <c r="K2" s="1">
+        <v>21.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="E1">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" s="1">
+        <v>50.06</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.96</v>
+      </c>
+      <c r="F3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G3" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="I3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" s="1">
+        <v>51.11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>17.03</v>
+      </c>
+      <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G4" s="1">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
+        <v>52.4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5.43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
+      <c r="C6" s="1">
+        <v>50.26</v>
+      </c>
+      <c r="D6" s="1">
+        <v>19.02</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added exclusivity to the genetic algorithm, fixed wheel roulette in a selection, fixed some bugs in a simulated annealing algorithm, fixed bug in a data reader, refactored lombok annotations, added second dataset
</commit_message>
<xml_diff>
--- a/input/Data.xlsx
+++ b/input/Data.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Data1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>V1</t>
   </si>
@@ -68,6 +69,171 @@
   </si>
   <si>
     <t>City name of depot</t>
+  </si>
+  <si>
+    <t>Gdansk</t>
+  </si>
+  <si>
+    <t>Szczecin</t>
+  </si>
+  <si>
+    <t>Bydgoszcz</t>
+  </si>
+  <si>
+    <t>Lublin</t>
+  </si>
+  <si>
+    <t>Bialystok</t>
+  </si>
+  <si>
+    <t>Gdynia</t>
+  </si>
+  <si>
+    <t>Czestochowa</t>
+  </si>
+  <si>
+    <t>Sosnowiec</t>
+  </si>
+  <si>
+    <t>Radom</t>
+  </si>
+  <si>
+    <t>Kielce</t>
+  </si>
+  <si>
+    <t>Torun</t>
+  </si>
+  <si>
+    <t>Gliwice</t>
+  </si>
+  <si>
+    <t>Zabrze</t>
+  </si>
+  <si>
+    <t>Bytom</t>
+  </si>
+  <si>
+    <t>Bielsko-biala</t>
+  </si>
+  <si>
+    <t>Olsztyn</t>
+  </si>
+  <si>
+    <t>Rzeszow</t>
+  </si>
+  <si>
+    <t>Ruda slaska</t>
+  </si>
+  <si>
+    <t>Rybnik</t>
+  </si>
+  <si>
+    <t>Tychy</t>
+  </si>
+  <si>
+    <t>Dabrowa gornicza</t>
+  </si>
+  <si>
+    <t>Walbrzych</t>
+  </si>
+  <si>
+    <t>Opole</t>
+  </si>
+  <si>
+    <t>Plock</t>
+  </si>
+  <si>
+    <t>Elblag</t>
+  </si>
+  <si>
+    <t>Gorzow wielkopolski</t>
+  </si>
+  <si>
+    <t>Wloclawek</t>
+  </si>
+  <si>
+    <t>Tarnow</t>
+  </si>
+  <si>
+    <t>Zielona gora</t>
+  </si>
+  <si>
+    <t>Chorzow</t>
+  </si>
+  <si>
+    <t>Kalisz</t>
+  </si>
+  <si>
+    <t>Koszalin</t>
+  </si>
+  <si>
+    <t>Legnica</t>
+  </si>
+  <si>
+    <t>Grudziadz</t>
+  </si>
+  <si>
+    <t>Slupsk</t>
+  </si>
+  <si>
+    <t>Jaworzno</t>
+  </si>
+  <si>
+    <t>Jastrzebie-zdroj</t>
+  </si>
+  <si>
+    <t>Jelenia gora</t>
+  </si>
+  <si>
+    <t>Nowy sacz</t>
+  </si>
+  <si>
+    <t>Konin</t>
+  </si>
+  <si>
+    <t>Piotrkow trybunalski</t>
+  </si>
+  <si>
+    <t>Lubin</t>
+  </si>
+  <si>
+    <t>Inowroclaw</t>
+  </si>
+  <si>
+    <t>Siedlce</t>
+  </si>
+  <si>
+    <t>Myslowice</t>
+  </si>
+  <si>
+    <t>Pila</t>
+  </si>
+  <si>
+    <t>Ostrowiec swietokrzyski</t>
+  </si>
+  <si>
+    <t>Siemianowice slaskie</t>
+  </si>
+  <si>
+    <t>Ostrow wielkopolski</t>
+  </si>
+  <si>
+    <t>Pabianice</t>
+  </si>
+  <si>
+    <t>Stargard szczecinski</t>
+  </si>
+  <si>
+    <t>Gniezno</t>
+  </si>
+  <si>
+    <t>Glogow</t>
+  </si>
+  <si>
+    <t>Suwalki</t>
+  </si>
+  <si>
+    <t>Chelm</t>
   </si>
 </sst>
 </file>
@@ -104,10 +270,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -478,6 +645,7 @@
       <c r="G2" s="1">
         <v>4.9000000000000004</v>
       </c>
+      <c r="H2" s="3"/>
       <c r="I2" t="s">
         <v>11</v>
       </c>
@@ -582,4 +750,943 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>51.77</v>
+      </c>
+      <c r="D2" s="1">
+        <v>19.46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>100</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1">
+        <v>52.26</v>
+      </c>
+      <c r="K2" s="1">
+        <v>21.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>50.06</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>200</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>51.11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>17.03</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>400</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>52.4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>54.36</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18.64</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>53.43</v>
+      </c>
+      <c r="D7" s="1">
+        <v>14.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>53.12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>18.010000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>51.24</v>
+      </c>
+      <c r="D9" s="1">
+        <v>22.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>50.26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>53.14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>54.52</v>
+      </c>
+      <c r="D12" s="1">
+        <v>18.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50.81</v>
+      </c>
+      <c r="D13" s="1">
+        <v>19.13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>50.28</v>
+      </c>
+      <c r="D14" s="1">
+        <v>19.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>51.4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>21.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>50.89</v>
+      </c>
+      <c r="D16" s="1">
+        <v>20.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>53.02</v>
+      </c>
+      <c r="D17" s="1">
+        <v>18.61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>50.31</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18.670000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50.3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>18.78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>50.35</v>
+      </c>
+      <c r="D20" s="1">
+        <v>18.91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>49.82</v>
+      </c>
+      <c r="D21" s="1">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>53.78</v>
+      </c>
+      <c r="D22" s="1">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>50.05</v>
+      </c>
+      <c r="D23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>50.3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>18.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>50.1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>50.16</v>
+      </c>
+      <c r="D26" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>50.33</v>
+      </c>
+      <c r="D27" s="1">
+        <v>19.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>50.78</v>
+      </c>
+      <c r="D28" s="1">
+        <v>16.28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>50.68</v>
+      </c>
+      <c r="D29" s="1">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>52.55</v>
+      </c>
+      <c r="D30" s="1">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>54.18</v>
+      </c>
+      <c r="D31" s="1">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1">
+        <v>52.74</v>
+      </c>
+      <c r="D32" s="1">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1">
+        <v>52.66</v>
+      </c>
+      <c r="D33" s="1">
+        <v>19.059999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="1">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1">
+        <v>50.01</v>
+      </c>
+      <c r="D34" s="1">
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1">
+        <v>51.94</v>
+      </c>
+      <c r="D35" s="1">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="1">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1">
+        <v>50.3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>19.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
+        <v>51.77</v>
+      </c>
+      <c r="D37" s="1">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1">
+        <v>12</v>
+      </c>
+      <c r="C38" s="1">
+        <v>54.19</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16.18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1">
+        <v>51.21</v>
+      </c>
+      <c r="D39" s="1">
+        <v>16.16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="1">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1">
+        <v>53.49</v>
+      </c>
+      <c r="D40" s="1">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="1">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1">
+        <v>54.47</v>
+      </c>
+      <c r="D41" s="1">
+        <v>17.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="1">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1">
+        <v>50.21</v>
+      </c>
+      <c r="D42" s="1">
+        <v>19.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="1">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1">
+        <v>49.99</v>
+      </c>
+      <c r="D43" s="1">
+        <v>18.59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1">
+        <v>15</v>
+      </c>
+      <c r="C44" s="1">
+        <v>50.91</v>
+      </c>
+      <c r="D44" s="1">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1">
+        <v>49.63</v>
+      </c>
+      <c r="D45" s="1">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1">
+        <v>15</v>
+      </c>
+      <c r="C46" s="1">
+        <v>52.21</v>
+      </c>
+      <c r="D46" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="1">
+        <v>15</v>
+      </c>
+      <c r="C47" s="1">
+        <v>51.41</v>
+      </c>
+      <c r="D47" s="1">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="1">
+        <v>15</v>
+      </c>
+      <c r="C48" s="1">
+        <v>51.4</v>
+      </c>
+      <c r="D48" s="1">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="1">
+        <v>15</v>
+      </c>
+      <c r="C49" s="1">
+        <v>52.78</v>
+      </c>
+      <c r="D49" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="1">
+        <v>15</v>
+      </c>
+      <c r="C50" s="1">
+        <v>52.17</v>
+      </c>
+      <c r="D50" s="1">
+        <v>22.28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15</v>
+      </c>
+      <c r="C51" s="1">
+        <v>50.24</v>
+      </c>
+      <c r="D51" s="1">
+        <v>19.14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="1">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1">
+        <v>53.15</v>
+      </c>
+      <c r="D52" s="1">
+        <v>16.739999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="1">
+        <v>20</v>
+      </c>
+      <c r="C53" s="1">
+        <v>50.95</v>
+      </c>
+      <c r="D53" s="1">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="1">
+        <v>20</v>
+      </c>
+      <c r="C54" s="1">
+        <v>50.33</v>
+      </c>
+      <c r="D54" s="1">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1">
+        <v>20</v>
+      </c>
+      <c r="C55" s="1">
+        <v>51.66</v>
+      </c>
+      <c r="D55" s="1">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1">
+        <v>20</v>
+      </c>
+      <c r="C56" s="1">
+        <v>51.67</v>
+      </c>
+      <c r="D56" s="1">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="1">
+        <v>20</v>
+      </c>
+      <c r="C57" s="1">
+        <v>53.34</v>
+      </c>
+      <c r="D57" s="1">
+        <v>15.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="1">
+        <v>20</v>
+      </c>
+      <c r="C58" s="1">
+        <v>52.53</v>
+      </c>
+      <c r="D58" s="1">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="1">
+        <v>20</v>
+      </c>
+      <c r="C59" s="1">
+        <v>51.67</v>
+      </c>
+      <c r="D59" s="1">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="1">
+        <v>20</v>
+      </c>
+      <c r="C60" s="1">
+        <v>54.11</v>
+      </c>
+      <c r="D60" s="1">
+        <v>22.94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="1">
+        <v>20</v>
+      </c>
+      <c r="C61" s="1">
+        <v>51.14</v>
+      </c>
+      <c r="D61" s="1">
+        <v>23.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug in a tabu and simulated annealing algorithm and created a new sheet with testing data and wrote special method (generateStaticResult) only for debbuging
</commit_message>
<xml_diff>
--- a/input/Data.xlsx
+++ b/input/Data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
     <sheet name="Data2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data_STATIC" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="73">
   <si>
     <t>V1</t>
   </si>
@@ -578,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +758,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,4 +1690,942 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>51.77</v>
+      </c>
+      <c r="D2" s="1">
+        <v>19.46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>200</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1">
+        <v>52.26</v>
+      </c>
+      <c r="K2" s="1">
+        <v>21.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>50.06</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>250</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>51.11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>17.03</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>400</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>52.4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>54.36</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18.64</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>53.43</v>
+      </c>
+      <c r="D7" s="1">
+        <v>14.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>53.12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>18.010000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>51.24</v>
+      </c>
+      <c r="D9" s="1">
+        <v>22.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>50.26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>53.14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>54.52</v>
+      </c>
+      <c r="D12" s="1">
+        <v>18.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50.81</v>
+      </c>
+      <c r="D13" s="1">
+        <v>19.13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>50.28</v>
+      </c>
+      <c r="D14" s="1">
+        <v>19.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>51.4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>21.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>50.89</v>
+      </c>
+      <c r="D16" s="1">
+        <v>20.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>53.02</v>
+      </c>
+      <c r="D17" s="1">
+        <v>18.61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>50.31</v>
+      </c>
+      <c r="D18" s="1">
+        <v>18.670000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50.3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>18.78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>50.35</v>
+      </c>
+      <c r="D20" s="1">
+        <v>18.91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>49.82</v>
+      </c>
+      <c r="D21" s="1">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>53.78</v>
+      </c>
+      <c r="D22" s="1">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>50.05</v>
+      </c>
+      <c r="D23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>50.3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>18.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>50.1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>50.16</v>
+      </c>
+      <c r="D26" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>50.33</v>
+      </c>
+      <c r="D27" s="1">
+        <v>19.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>50.78</v>
+      </c>
+      <c r="D28" s="1">
+        <v>16.28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>50.68</v>
+      </c>
+      <c r="D29" s="1">
+        <v>17.940000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>52.55</v>
+      </c>
+      <c r="D30" s="1">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>54.18</v>
+      </c>
+      <c r="D31" s="1">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1">
+        <v>52.74</v>
+      </c>
+      <c r="D32" s="1">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1">
+        <v>52.66</v>
+      </c>
+      <c r="D33" s="1">
+        <v>19.059999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="1">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1">
+        <v>50.01</v>
+      </c>
+      <c r="D34" s="1">
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1">
+        <v>51.94</v>
+      </c>
+      <c r="D35" s="1">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="1">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1">
+        <v>50.3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>19.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
+        <v>51.77</v>
+      </c>
+      <c r="D37" s="1">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1">
+        <v>12</v>
+      </c>
+      <c r="C38" s="1">
+        <v>54.19</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16.18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1">
+        <v>51.21</v>
+      </c>
+      <c r="D39" s="1">
+        <v>16.16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="1">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1">
+        <v>53.49</v>
+      </c>
+      <c r="D40" s="1">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="1">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1">
+        <v>54.47</v>
+      </c>
+      <c r="D41" s="1">
+        <v>17.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="1">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1">
+        <v>50.21</v>
+      </c>
+      <c r="D42" s="1">
+        <v>19.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="1">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1">
+        <v>49.99</v>
+      </c>
+      <c r="D43" s="1">
+        <v>18.59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1">
+        <v>15</v>
+      </c>
+      <c r="C44" s="1">
+        <v>50.91</v>
+      </c>
+      <c r="D44" s="1">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1">
+        <v>49.63</v>
+      </c>
+      <c r="D45" s="1">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1">
+        <v>15</v>
+      </c>
+      <c r="C46" s="1">
+        <v>52.21</v>
+      </c>
+      <c r="D46" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="1">
+        <v>15</v>
+      </c>
+      <c r="C47" s="1">
+        <v>51.41</v>
+      </c>
+      <c r="D47" s="1">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="1">
+        <v>15</v>
+      </c>
+      <c r="C48" s="1">
+        <v>51.4</v>
+      </c>
+      <c r="D48" s="1">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="1">
+        <v>15</v>
+      </c>
+      <c r="C49" s="1">
+        <v>52.78</v>
+      </c>
+      <c r="D49" s="1">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="1">
+        <v>15</v>
+      </c>
+      <c r="C50" s="1">
+        <v>52.17</v>
+      </c>
+      <c r="D50" s="1">
+        <v>22.28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15</v>
+      </c>
+      <c r="C51" s="1">
+        <v>50.24</v>
+      </c>
+      <c r="D51" s="1">
+        <v>19.14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="1">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1">
+        <v>53.15</v>
+      </c>
+      <c r="D52" s="1">
+        <v>16.739999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="1">
+        <v>20</v>
+      </c>
+      <c r="C53" s="1">
+        <v>50.95</v>
+      </c>
+      <c r="D53" s="1">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="1">
+        <v>20</v>
+      </c>
+      <c r="C54" s="1">
+        <v>50.33</v>
+      </c>
+      <c r="D54" s="1">
+        <v>19.05</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="1">
+        <v>20</v>
+      </c>
+      <c r="C55" s="1">
+        <v>51.66</v>
+      </c>
+      <c r="D55" s="1">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1">
+        <v>20</v>
+      </c>
+      <c r="C56" s="1">
+        <v>51.67</v>
+      </c>
+      <c r="D56" s="1">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="1">
+        <v>20</v>
+      </c>
+      <c r="C57" s="1">
+        <v>53.34</v>
+      </c>
+      <c r="D57" s="1">
+        <v>15.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="1">
+        <v>20</v>
+      </c>
+      <c r="C58" s="1">
+        <v>52.53</v>
+      </c>
+      <c r="D58" s="1">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="1">
+        <v>20</v>
+      </c>
+      <c r="C59" s="1">
+        <v>51.67</v>
+      </c>
+      <c r="D59" s="1">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="1">
+        <v>20</v>
+      </c>
+      <c r="C60" s="1">
+        <v>54.11</v>
+      </c>
+      <c r="D60" s="1">
+        <v>22.94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="1">
+        <v>20</v>
+      </c>
+      <c r="C61" s="1">
+        <v>51.14</v>
+      </c>
+      <c r="D61" s="1">
+        <v>23.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactored genetic algorithm: changed decoding and encoding, added partial mapped crossover
</commit_message>
<xml_diff>
--- a/input/Data.xlsx
+++ b/input/Data.xlsx
@@ -9,14 +9,15 @@
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
     <sheet name="Data2" sheetId="2" r:id="rId2"/>
-    <sheet name="Data_STATIC" sheetId="4" r:id="rId3"/>
+    <sheet name="Data3" sheetId="5" r:id="rId3"/>
+    <sheet name="Data_STATIC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="73">
   <si>
     <t>V1</t>
   </si>
@@ -758,7 +759,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B55" sqref="B55:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,9 +1695,259 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>51.77</v>
+      </c>
+      <c r="D2" s="1">
+        <v>19.46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1">
+        <v>52.26</v>
+      </c>
+      <c r="K2" s="1">
+        <v>21.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>50.06</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>51.11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>17.03</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>52.4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>54.36</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18.64</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>53.43</v>
+      </c>
+      <c r="D7" s="1">
+        <v>14.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>53.12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>18.010000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>51.24</v>
+      </c>
+      <c r="D9" s="1">
+        <v>22.57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>50.26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
prepared data input and fixed bug in a reading sheets from file
</commit_message>
<xml_diff>
--- a/input/Data.xlsx
+++ b/input/Data.xlsx
@@ -4,21 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="13395" windowHeight="7245"/>
   </bookViews>
   <sheets>
     <sheet name="Data60" sheetId="7" r:id="rId1"/>
     <sheet name="Data80" sheetId="9" r:id="rId2"/>
     <sheet name="Data100" sheetId="10" r:id="rId3"/>
     <sheet name="Europe" sheetId="8" r:id="rId4"/>
-    <sheet name="WrongData" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="308">
   <si>
     <t>V1</t>
   </si>
@@ -942,18 +941,6 @@
   </si>
   <si>
     <t>V5</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -5507,7 +5494,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:G12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6320,75 +6307,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F2" t="s">
-        <v>310</v>
-      </c>
-      <c r="G2" t="s">
-        <v>311</v>
-      </c>
-      <c r="H2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="O28" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
-        <v>311</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>